<commit_message>
sections organised and aligned with the classification of the table of activities
</commit_message>
<xml_diff>
--- a/Data/CB_activities_2025.xlsx
+++ b/Data/CB_activities_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfernandez diaz\Documents\DATA SECTION\Meetings\2025\WPDCS21\iotc-data-section-activities\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1801CF-40AE-4FE9-AE91-9ABF6A8A7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA63C8BE-C6D4-49D1-8C05-45BC05D0E442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D41A8BB6-56DB-424A-9F0C-BE9C289580A7}"/>
   </bookViews>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06C795F-10D4-45CE-959B-82C1D2A020ED}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1680,8 +1680,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>18</v>
+      <c r="A14" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>5</v>
@@ -1700,8 +1700,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
+      <c r="A15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>4</v>

</xml_diff>